<commit_message>
added util hrs and total hrs display
</commit_message>
<xml_diff>
--- a/data/TEST/sample_checksheet.xlsx
+++ b/data/TEST/sample_checksheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21267" windowHeight="8019" activeTab="2"/>
+    <workbookView windowWidth="21267" windowHeight="7299" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="F15" sheetId="1" r:id="rId1"/>
@@ -1890,7 +1890,7 @@
   <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="G5" sqref="G5:I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.79279279279279" defaultRowHeight="14.4"/>
@@ -2005,9 +2005,16 @@
         <v>5</v>
       </c>
       <c r="F5" s="11"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
+      <c r="G5" s="12">
+        <v>123</v>
+      </c>
+      <c r="H5" s="12">
+        <v>130</v>
+      </c>
+      <c r="I5" s="12">
+        <f>H5-G5</f>
+        <v>7</v>
+      </c>
       <c r="J5" s="9">
         <v>20113</v>
       </c>
@@ -2030,9 +2037,16 @@
         <v>0</v>
       </c>
       <c r="F6" s="11"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
+      <c r="G6" s="12">
+        <v>230</v>
+      </c>
+      <c r="H6" s="12">
+        <v>231</v>
+      </c>
+      <c r="I6" s="12">
+        <f t="shared" ref="I6:I18" si="0">H6-G6</f>
+        <v>1</v>
+      </c>
       <c r="J6" s="61">
         <v>20140</v>
       </c>
@@ -2055,9 +2069,16 @@
         <v>0</v>
       </c>
       <c r="F7" s="11"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
+      <c r="G7" s="12">
+        <v>22</v>
+      </c>
+      <c r="H7" s="12">
+        <v>34</v>
+      </c>
+      <c r="I7" s="12">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
       <c r="J7" s="61">
         <v>23018</v>
       </c>
@@ -2080,9 +2101,16 @@
         <v>0</v>
       </c>
       <c r="F8" s="11"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
+      <c r="G8" s="12">
+        <v>109</v>
+      </c>
+      <c r="H8" s="12">
+        <v>119</v>
+      </c>
+      <c r="I8" s="12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="J8" s="61">
         <v>23130</v>
       </c>
@@ -2105,9 +2133,16 @@
         <v>0</v>
       </c>
       <c r="F9" s="11"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
+      <c r="G9" s="12">
+        <v>110</v>
+      </c>
+      <c r="H9" s="12">
+        <v>120</v>
+      </c>
+      <c r="I9" s="12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="J9" s="61">
         <v>23321</v>
       </c>
@@ -2130,9 +2165,16 @@
         <v>0</v>
       </c>
       <c r="F10" s="11"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
+      <c r="G10" s="12">
+        <v>111</v>
+      </c>
+      <c r="H10" s="12">
+        <v>121</v>
+      </c>
+      <c r="I10" s="12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="J10" s="61">
         <v>25122</v>
       </c>
@@ -2155,9 +2197,16 @@
         <v>0</v>
       </c>
       <c r="F11" s="11"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
+      <c r="G11" s="12">
+        <v>112</v>
+      </c>
+      <c r="H11" s="12">
+        <v>122</v>
+      </c>
+      <c r="I11" s="12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="J11" s="61">
         <v>25124</v>
       </c>
@@ -2180,9 +2229,16 @@
         <v>0</v>
       </c>
       <c r="F12" s="11"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
+      <c r="G12" s="12">
+        <v>113</v>
+      </c>
+      <c r="H12" s="12">
+        <v>123</v>
+      </c>
+      <c r="I12" s="12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="J12" s="61">
         <v>25225</v>
       </c>
@@ -2205,9 +2261,16 @@
         <v>0</v>
       </c>
       <c r="F13" s="11"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
+      <c r="G13" s="12">
+        <v>114</v>
+      </c>
+      <c r="H13" s="12">
+        <v>124</v>
+      </c>
+      <c r="I13" s="12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="J13" s="61">
         <v>25231</v>
       </c>
@@ -2230,9 +2293,16 @@
         <v>0</v>
       </c>
       <c r="F14" s="11"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
+      <c r="G14" s="12">
+        <v>115</v>
+      </c>
+      <c r="H14" s="12">
+        <v>125</v>
+      </c>
+      <c r="I14" s="12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="J14" s="61">
         <v>25522</v>
       </c>
@@ -2255,9 +2325,16 @@
         <v>0</v>
       </c>
       <c r="F15" s="11"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
+      <c r="G15" s="12">
+        <v>763</v>
+      </c>
+      <c r="H15" s="12">
+        <v>799</v>
+      </c>
+      <c r="I15" s="12">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
       <c r="J15" s="61">
         <v>25731</v>
       </c>
@@ -2280,9 +2357,16 @@
         <v>0</v>
       </c>
       <c r="F16" s="11"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
+      <c r="G16" s="12">
+        <v>77</v>
+      </c>
+      <c r="H16" s="12">
+        <v>80</v>
+      </c>
+      <c r="I16" s="12">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
       <c r="J16" s="61">
         <v>25820</v>
       </c>
@@ -2305,9 +2389,16 @@
         <v>0</v>
       </c>
       <c r="F17" s="11"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
+      <c r="G17" s="12">
+        <v>90</v>
+      </c>
+      <c r="H17" s="12">
+        <v>95</v>
+      </c>
+      <c r="I17" s="12">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
       <c r="J17" s="61">
         <v>25965</v>
       </c>
@@ -2330,9 +2421,16 @@
         <v>0</v>
       </c>
       <c r="F18" s="11"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
+      <c r="G18" s="12">
+        <v>120</v>
+      </c>
+      <c r="H18" s="12">
+        <v>125</v>
+      </c>
+      <c r="I18" s="12">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
       <c r="J18" s="9">
         <v>25969</v>
       </c>
@@ -2732,8 +2830,8 @@
   <sheetPr/>
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.79279279279279" defaultRowHeight="14.4"/>
@@ -2848,9 +2946,16 @@
         <v>0</v>
       </c>
       <c r="F5" s="11"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
+      <c r="G5" s="12">
+        <v>123</v>
+      </c>
+      <c r="H5" s="12">
+        <v>130</v>
+      </c>
+      <c r="I5" s="12">
+        <f t="shared" ref="I5:I18" si="0">H5-G5</f>
+        <v>7</v>
+      </c>
       <c r="J5" s="51">
         <v>20140</v>
       </c>
@@ -2873,9 +2978,16 @@
         <v>0</v>
       </c>
       <c r="F6" s="11"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
+      <c r="G6" s="12">
+        <v>230</v>
+      </c>
+      <c r="H6" s="12">
+        <v>231</v>
+      </c>
+      <c r="I6" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="J6" s="51">
         <v>20240</v>
       </c>
@@ -2898,9 +3010,16 @@
         <v>0</v>
       </c>
       <c r="F7" s="11"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
+      <c r="G7" s="12">
+        <v>22</v>
+      </c>
+      <c r="H7" s="12">
+        <v>34</v>
+      </c>
+      <c r="I7" s="12">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
       <c r="J7" s="51">
         <v>20260</v>
       </c>
@@ -2923,9 +3042,16 @@
         <v>0</v>
       </c>
       <c r="F8" s="11"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
+      <c r="G8" s="12">
+        <v>109</v>
+      </c>
+      <c r="H8" s="12">
+        <v>119</v>
+      </c>
+      <c r="I8" s="12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="J8" s="51">
         <v>23018</v>
       </c>
@@ -2948,9 +3074,16 @@
         <v>0</v>
       </c>
       <c r="F9" s="11"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
+      <c r="G9" s="12">
+        <v>110</v>
+      </c>
+      <c r="H9" s="12">
+        <v>120</v>
+      </c>
+      <c r="I9" s="12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="J9" s="51">
         <v>23321</v>
       </c>
@@ -2973,9 +3106,16 @@
         <v>0</v>
       </c>
       <c r="F10" s="11"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
+      <c r="G10" s="12">
+        <v>111</v>
+      </c>
+      <c r="H10" s="12">
+        <v>121</v>
+      </c>
+      <c r="I10" s="12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="J10" s="51">
         <v>25122</v>
       </c>
@@ -2998,9 +3138,16 @@
         <v>0</v>
       </c>
       <c r="F11" s="11"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
+      <c r="G11" s="12">
+        <v>112</v>
+      </c>
+      <c r="H11" s="12">
+        <v>122</v>
+      </c>
+      <c r="I11" s="12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="J11" s="51">
         <v>25231</v>
       </c>
@@ -3023,9 +3170,16 @@
         <v>0</v>
       </c>
       <c r="F12" s="11"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
+      <c r="G12" s="12">
+        <v>113</v>
+      </c>
+      <c r="H12" s="12">
+        <v>123</v>
+      </c>
+      <c r="I12" s="12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="J12" s="51">
         <v>25931</v>
       </c>
@@ -3048,9 +3202,16 @@
         <v>0</v>
       </c>
       <c r="F13" s="11"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
+      <c r="G13" s="12">
+        <v>114</v>
+      </c>
+      <c r="H13" s="12">
+        <v>124</v>
+      </c>
+      <c r="I13" s="12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="J13" s="51">
         <v>25965</v>
       </c>
@@ -3073,9 +3234,16 @@
         <v>0</v>
       </c>
       <c r="F14" s="11"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
+      <c r="G14" s="12">
+        <v>115</v>
+      </c>
+      <c r="H14" s="12">
+        <v>125</v>
+      </c>
+      <c r="I14" s="12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="J14" s="51">
         <v>25969</v>
       </c>
@@ -3098,9 +3266,16 @@
         <v>3</v>
       </c>
       <c r="F15" s="11"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
+      <c r="G15" s="12">
+        <v>763</v>
+      </c>
+      <c r="H15" s="12">
+        <v>799</v>
+      </c>
+      <c r="I15" s="12">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
       <c r="J15" s="9">
         <v>20113</v>
       </c>
@@ -3545,8 +3720,8 @@
   <sheetPr/>
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="G16:J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.79279279279279" defaultRowHeight="14.4"/>
@@ -3661,9 +3836,16 @@
         <v>0</v>
       </c>
       <c r="F5" s="11"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
+      <c r="G5" s="12">
+        <v>123</v>
+      </c>
+      <c r="H5" s="12">
+        <v>130</v>
+      </c>
+      <c r="I5" s="12">
+        <f t="shared" ref="I5:I18" si="0">H5-G5</f>
+        <v>7</v>
+      </c>
       <c r="J5" s="50">
         <v>20240</v>
       </c>
@@ -3686,9 +3868,16 @@
         <v>0</v>
       </c>
       <c r="F6" s="11"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
+      <c r="G6" s="12">
+        <v>230</v>
+      </c>
+      <c r="H6" s="12">
+        <v>231</v>
+      </c>
+      <c r="I6" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="J6" s="50">
         <v>23018</v>
       </c>
@@ -3711,9 +3900,16 @@
         <v>0</v>
       </c>
       <c r="F7" s="11"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
+      <c r="G7" s="12">
+        <v>22</v>
+      </c>
+      <c r="H7" s="12">
+        <v>34</v>
+      </c>
+      <c r="I7" s="12">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
       <c r="J7" s="51">
         <v>23321</v>
       </c>
@@ -3736,9 +3932,16 @@
         <v>0</v>
       </c>
       <c r="F8" s="11"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
+      <c r="G8" s="12">
+        <v>109</v>
+      </c>
+      <c r="H8" s="12">
+        <v>119</v>
+      </c>
+      <c r="I8" s="12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="J8" s="51">
         <v>25121</v>
       </c>
@@ -3761,9 +3964,16 @@
         <v>0</v>
       </c>
       <c r="F9" s="11"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
+      <c r="G9" s="12">
+        <v>110</v>
+      </c>
+      <c r="H9" s="12">
+        <v>120</v>
+      </c>
+      <c r="I9" s="12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="J9" s="51">
         <v>25122</v>
       </c>
@@ -3786,9 +3996,16 @@
         <v>0</v>
       </c>
       <c r="F10" s="11"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
+      <c r="G10" s="12">
+        <v>111</v>
+      </c>
+      <c r="H10" s="12">
+        <v>121</v>
+      </c>
+      <c r="I10" s="12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="J10" s="51">
         <v>25223</v>
       </c>
@@ -3811,9 +4028,16 @@
         <v>0</v>
       </c>
       <c r="F11" s="11"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
+      <c r="G11" s="12">
+        <v>112</v>
+      </c>
+      <c r="H11" s="12">
+        <v>122</v>
+      </c>
+      <c r="I11" s="12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="J11" s="51">
         <v>25320</v>
       </c>
@@ -3836,9 +4060,16 @@
         <v>0</v>
       </c>
       <c r="F12" s="11"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
+      <c r="G12" s="12">
+        <v>113</v>
+      </c>
+      <c r="H12" s="12">
+        <v>123</v>
+      </c>
+      <c r="I12" s="12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="J12" s="51">
         <v>25325</v>
       </c>
@@ -3861,9 +4092,16 @@
         <v>0</v>
       </c>
       <c r="F13" s="11"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
+      <c r="G13" s="12">
+        <v>114</v>
+      </c>
+      <c r="H13" s="12">
+        <v>124</v>
+      </c>
+      <c r="I13" s="12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="J13" s="51">
         <v>25934</v>
       </c>
@@ -3886,9 +4124,16 @@
         <v>0</v>
       </c>
       <c r="F14" s="11"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
+      <c r="G14" s="12">
+        <v>115</v>
+      </c>
+      <c r="H14" s="12">
+        <v>125</v>
+      </c>
+      <c r="I14" s="12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="J14" s="51">
         <v>25966</v>
       </c>
@@ -3911,9 +4156,16 @@
         <v>7</v>
       </c>
       <c r="F15" s="11"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
+      <c r="G15" s="12">
+        <v>763</v>
+      </c>
+      <c r="H15" s="12">
+        <v>799</v>
+      </c>
+      <c r="I15" s="12">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
       <c r="J15" s="9">
         <v>20113</v>
       </c>

</xml_diff>